<commit_message>
Tables and graphs before presentation
</commit_message>
<xml_diff>
--- a/data/tables.xlsx
+++ b/data/tables.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/tourism/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE8EFF47-2312-E943-BF43-368F5EE8A9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B72242-4FA2-2545-9573-BD30B4818017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29200" windowHeight="15920" activeTab="7" xr2:uid="{AFF4729F-041D-4372-8C6D-3246B2E7546E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19700" activeTab="6" xr2:uid="{AFF4729F-041D-4372-8C6D-3246B2E7546E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table &quot;exporters&quot;" sheetId="1" r:id="rId1"/>
-    <sheet name="Table &quot;importers&quot;" sheetId="2" r:id="rId2"/>
-    <sheet name="Table_transp" sheetId="4" r:id="rId3"/>
-    <sheet name="Table_large travel" sheetId="3" r:id="rId4"/>
-    <sheet name="Table_CA_2019" sheetId="5" r:id="rId5"/>
-    <sheet name="Table_GDPPC-IIP_2019" sheetId="6" r:id="rId6"/>
-    <sheet name="Chart_adjust_2020" sheetId="8" r:id="rId7"/>
-    <sheet name="Data_adjustment" sheetId="7" r:id="rId8"/>
+    <sheet name="Table 1_large travel" sheetId="3" r:id="rId1"/>
+    <sheet name="Table 2A &quot;exporters&quot;" sheetId="1" r:id="rId2"/>
+    <sheet name="Table 2B &quot;importers&quot;" sheetId="2" r:id="rId3"/>
+    <sheet name="Table 3_CA_2019" sheetId="5" r:id="rId4"/>
+    <sheet name="Table 4_GDPPC-IIP_2019" sheetId="6" r:id="rId5"/>
+    <sheet name="Table_5_transp" sheetId="4" r:id="rId6"/>
+    <sheet name="Table_6_tourism" sheetId="10" r:id="rId7"/>
+    <sheet name="tourism_tidy" sheetId="11" r:id="rId8"/>
+    <sheet name="surprise_tidy" sheetId="12" r:id="rId9"/>
+    <sheet name="Fig_2_adjust_2020" sheetId="8" r:id="rId10"/>
+    <sheet name="Data_adjustment" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="130">
   <si>
     <t>billions USD</t>
   </si>
@@ -356,6 +359,81 @@
   </si>
   <si>
     <t>Size and creditor position: tourism-dependent economies and other economies</t>
+  </si>
+  <si>
+    <t>balance on secondary income</t>
+  </si>
+  <si>
+    <t>All countries</t>
+  </si>
+  <si>
+    <t>Share of tourism in GDP (average, 2015-19): stylized facts</t>
+  </si>
+  <si>
+    <t>75th perc.</t>
+  </si>
+  <si>
+    <t>25th perc.</t>
+  </si>
+  <si>
+    <t>Obs.</t>
+  </si>
+  <si>
+    <t>Std. dev.</t>
+  </si>
+  <si>
+    <t>Direct share</t>
+  </si>
+  <si>
+    <t>Total share</t>
+  </si>
+  <si>
+    <t>Adv. Ec.</t>
+  </si>
+  <si>
+    <t>Emg. and Dev. Ec.</t>
+  </si>
+  <si>
+    <t>tourism</t>
+  </si>
+  <si>
+    <t>country_group</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>q25</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>q75</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>Advanced economics</t>
+  </si>
+  <si>
+    <t>Emerging and developing economies</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -365,7 +443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,8 +486,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +510,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -455,7 +552,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -516,6 +613,16 @@
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -525,6 +632,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +779,7 @@
                   <c:v>Balance on primary income</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Balance on secondary income</c:v>
+                  <c:v>balance on secondary income</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1401,7 +1517,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E0260D30-DA38-4E4C-B57E-1AF7B7B63B0D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1412,7 +1528,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8680275" cy="6291743"/>
+    <xdr:ext cx="8663983" cy="6285424"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1737,11 +1853,891 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9A4C79-82CA-4BF3-8CF0-A42D32042EC4}">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4">
+        <v>67.930134460146263</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="D3" s="4">
+        <v>55.154034599635715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4">
+        <v>54.422865772358897</v>
+      </c>
+      <c r="C4" s="1">
+        <v>7.7142000000000002E-2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3.1551076475507958</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4">
+        <v>51.874196341724712</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.372</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5.6319177003723295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4">
+        <v>48.78376973831292</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.112</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3.3416341739058324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="4">
+        <v>46.310440110633465</v>
+      </c>
+      <c r="C7" s="1">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.6619592592592591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="4">
+        <v>42.690670934685158</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.1187915464671665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4">
+        <v>40.933380524003205</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.112</v>
+      </c>
+      <c r="D9" s="4">
+        <v>1.2050169994221624</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="4">
+        <v>37.80357401561308</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.28042940625000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4">
+        <v>29.184731185530865</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.1639085744788999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="4">
+        <v>28.808808649853312</v>
+      </c>
+      <c r="C12" s="1">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.5800768394649225</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="4">
+        <v>28.029657202706129</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.92359608895041967</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4">
+        <v>24.957625968211211</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.82471851851851841</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="4">
+        <v>24.19915495212669</v>
+      </c>
+      <c r="C15" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.57852048148148139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="4">
+        <v>23.426060338983973</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="D16" s="4">
+        <v>13.578799999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4">
+        <v>20.970349597414291</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.9825185406134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4">
+        <v>20.519983638199051</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.623</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5.5428131458303209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="4">
+        <v>20.518964002216507</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.85225658584127795</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="4">
+        <v>19.655198810262576</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5.2979588617104501</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="4">
+        <v>18.863590913688778</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1.9818461711964659</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="4">
+        <v>17.526765654825013</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2.734</v>
+      </c>
+      <c r="D22" s="4">
+        <v>15.807932888968995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="4">
+        <v>15.615972357211408</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.0679999999999996</v>
+      </c>
+      <c r="D23" s="4">
+        <v>60.752171540493542</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="4">
+        <v>15.039183722225999</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="D24" s="4">
+        <v>5.4972580042428421</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="4">
+        <v>13.861384589203558</v>
+      </c>
+      <c r="C25" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="D25" s="4">
+        <v>26.727593461374745</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="4">
+        <v>13.149106851576454</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3.7240000000000002</v>
+      </c>
+      <c r="D26" s="4">
+        <v>17.476842102993885</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="4">
+        <v>12.441988834685356</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.4218140803669676</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="4">
+        <v>12.393707069492546</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="D28" s="4">
+        <v>7.9533552117448307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="4">
+        <v>9.122894701715115</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="D29" s="4">
+        <v>15.214920017147165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="4">
+        <v>8.7262991641330387</v>
+      </c>
+      <c r="C30" s="1">
+        <v>69.626000000000005</v>
+      </c>
+      <c r="D30" s="4">
+        <v>544.20954952918362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="4">
+        <v>8.2046387247601285</v>
+      </c>
+      <c r="C31" s="1">
+        <v>10.07</v>
+      </c>
+      <c r="D31" s="4">
+        <v>44.565751751798686</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="4">
+        <v>8.1907939958705605</v>
+      </c>
+      <c r="C32" s="1">
+        <v>1.2669999999999999</v>
+      </c>
+      <c r="D32" s="4">
+        <v>14.048423918124824</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="4">
+        <v>8.0623293936444256</v>
+      </c>
+      <c r="C33" s="1">
+        <v>10.358000000000001</v>
+      </c>
+      <c r="D33" s="4">
+        <v>89.031619777110421</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="4">
+        <v>7.6027123016297669</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.876</v>
+      </c>
+      <c r="D34" s="4">
+        <v>24.952593909616546</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="4">
+        <v>7.3461562244860756</v>
+      </c>
+      <c r="C35" s="1">
+        <v>10.725</v>
+      </c>
+      <c r="D35" s="4">
+        <v>205.34883886842613</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="4">
+        <v>5.5386213839232239</v>
+      </c>
+      <c r="C36" s="1">
+        <v>10.286</v>
+      </c>
+      <c r="D36" s="4">
+        <v>239.53710912982544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="4">
+        <v>5.2515834542103743</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4.2190000000000003</v>
+      </c>
+      <c r="D37" s="4">
+        <v>66.787866841095592</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="4">
+        <v>5.2090756832364296</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1.484</v>
+      </c>
+      <c r="D38" s="4">
+        <v>38.473723404255317</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5.1634574951397969</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="D39" s="4">
+        <v>24.836710978851144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" s="4">
+        <f>AVERAGE(B3:B39)</f>
+        <v>22.387292669152441</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" ref="C41:D41" si="0">AVERAGE(C3:C39)</f>
+        <v>4.1493011351351354</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="0"/>
+        <v>41.851350825853245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="4">
+        <f>MEDIAN(B3:B39)</f>
+        <v>18.863590913688778</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" ref="C42:D42" si="1">MEDIAN(C3:C39)</f>
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="1"/>
+        <v>5.6319177003723295</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="9"/>
+      <c r="D43" s="10"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="10"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="4">
+        <v>64.756210402315816</v>
+      </c>
+      <c r="C45" s="1">
+        <v>5.8559999999999999</v>
+      </c>
+      <c r="D45" s="4">
+        <v>1.1974200000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="4">
+        <v>60.207974676378726</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4.1486000000000002E-2</v>
+      </c>
+      <c r="D46" s="4">
+        <v>1.0089999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="4">
+        <v>38.940448139497711</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1.4730999999999999E-2</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0.37958518518518519</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="4">
+        <v>11.317765119694657</v>
+      </c>
+      <c r="C48" s="1">
+        <v>6.4173999999999995E-2</v>
+      </c>
+      <c r="D48" s="4">
+        <v>6.0201840000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="4">
+        <v>7.8640318001519294</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.16342400000000001</v>
+      </c>
+      <c r="D49" s="4">
+        <v>3.1017877094972</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="4">
+        <v>6.0610415390536456</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.27928399999999998</v>
+      </c>
+      <c r="D50" s="4">
+        <v>6.02336768898674</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9F6483-098D-4B3D-8661-531F940D7152}">
+  <dimension ref="A2:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="10">
+        <v>-4.7584939999999998</v>
+      </c>
+      <c r="C4" s="10">
+        <v>5.3715250000000001</v>
+      </c>
+      <c r="D4" s="10">
+        <v>-4.8007220000000004</v>
+      </c>
+      <c r="E4" s="10">
+        <v>-15.45575</v>
+      </c>
+      <c r="F4" s="10">
+        <v>9.3905700000000003</v>
+      </c>
+      <c r="G4" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2.5102600000000002</v>
+      </c>
+      <c r="C5" s="10">
+        <v>3.1506069999999999</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1.8544849999999999</v>
+      </c>
+      <c r="E5" s="10">
+        <v>-4.2025220000000001</v>
+      </c>
+      <c r="F5" s="10">
+        <v>8.4722139999999992</v>
+      </c>
+      <c r="G5" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="10">
+        <v>1.36439</v>
+      </c>
+      <c r="C6" s="10">
+        <v>4.0988309999999997</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.18954109999999999</v>
+      </c>
+      <c r="E6" s="10">
+        <v>-4.4756530000000003</v>
+      </c>
+      <c r="F6" s="10">
+        <v>17.131250000000001</v>
+      </c>
+      <c r="G6" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="10">
+        <v>-11.470890000000001</v>
+      </c>
+      <c r="C7" s="10">
+        <v>6.4548839999999998</v>
+      </c>
+      <c r="D7" s="10">
+        <v>-10.673719999999999</v>
+      </c>
+      <c r="E7" s="10">
+        <v>-23.69586</v>
+      </c>
+      <c r="F7" s="10">
+        <v>-0.96835139999999997</v>
+      </c>
+      <c r="G7" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1.38619</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2.0649359999999999</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1.0368250000000001</v>
+      </c>
+      <c r="E8" s="10">
+        <v>-1.6213</v>
+      </c>
+      <c r="F8" s="10">
+        <v>7.4287510000000001</v>
+      </c>
+      <c r="G8" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1.4515629999999999</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2.187506</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.80064999999999997</v>
+      </c>
+      <c r="E9" s="10">
+        <v>-2.7993000000000001</v>
+      </c>
+      <c r="F9" s="10">
+        <v>5.5223000000000004</v>
+      </c>
+      <c r="G9" s="13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9A6576-5B5D-4148-9969-188885C0292E}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1891,7 +2887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE40F65-0CEA-4BC5-8ED6-BB4FF0DBAFE8}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -2045,1392 +3041,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33FD584-3AA7-477E-8AE4-0DD69A91E032}">
-  <dimension ref="A1:B200"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="4">
-        <v>7.0160379932140611</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="4">
-        <v>5.9485074187079601</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="11">
-        <v>5.1204749911959739</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="4">
-        <v>4.9184804413390042</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="4">
-        <v>4.3485991674098523</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="4">
-        <v>3.7569446794271428</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="4">
-        <v>3.3441612719013563</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="4">
-        <v>3.2104974633661691</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="4">
-        <v>3.1652758935326522</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2.8373919457960826</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B62" s="1"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B63" s="1"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B64" s="1"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="1"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="1"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B67" s="1"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B68" s="1"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B70" s="1"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B72" s="1"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B74" s="1"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B76" s="1"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B77" s="1"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B78" s="1"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B84" s="1"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B85" s="1"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B86" s="1"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B87" s="1"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B88" s="1"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B89" s="1"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B90" s="1"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B92" s="1"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B93" s="1"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B95" s="1"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B96" s="1"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B97" s="1"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B98" s="1"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B99" s="1"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B100" s="1"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B101" s="1"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B102" s="1"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B103" s="1"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B104" s="1"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B105" s="1"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B106" s="1"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B107" s="1"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B108" s="1"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B109" s="1"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B110" s="1"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B111" s="1"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B112" s="1"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B113" s="1"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B114" s="1"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B115" s="1"/>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B116" s="1"/>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B117" s="1"/>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B119" s="1"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B120" s="1"/>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B121" s="1"/>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B122" s="1"/>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B123" s="1"/>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B124" s="8"/>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B125" s="1"/>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B126" s="1"/>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B127" s="1"/>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B128" s="1"/>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B129" s="1"/>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B130" s="1"/>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B131" s="1"/>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B132" s="1"/>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B133" s="1"/>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B134" s="1"/>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B135" s="1"/>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B136" s="1"/>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B137" s="1"/>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B138" s="1"/>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B139" s="1"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B140" s="1"/>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B141" s="1"/>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B142" s="1"/>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B143" s="1"/>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B144" s="1"/>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B145" s="1"/>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B146" s="1"/>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B147" s="1"/>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B148" s="1"/>
-    </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B149" s="1"/>
-    </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B150" s="1"/>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B151" s="1"/>
-    </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B152" s="1"/>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B153" s="1"/>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B154" s="1"/>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B155" s="1"/>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B156" s="1"/>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B157" s="1"/>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B158" s="1"/>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B159" s="1"/>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B160" s="1"/>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B161" s="1"/>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B162" s="1"/>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B163" s="1"/>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B164" s="1"/>
-    </row>
-    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B165" s="1"/>
-    </row>
-    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B166" s="1"/>
-    </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B167" s="1"/>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B168" s="1"/>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B169" s="1"/>
-    </row>
-    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B170" s="1"/>
-    </row>
-    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B171" s="1"/>
-    </row>
-    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B172" s="1"/>
-    </row>
-    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B173" s="1"/>
-    </row>
-    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B174" s="1"/>
-    </row>
-    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B175" s="1"/>
-    </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B176" s="1"/>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B177" s="1"/>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B178" s="1"/>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B179" s="1"/>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B180" s="1"/>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B181" s="1"/>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B182" s="1"/>
-    </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B183" s="1"/>
-    </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B184" s="1"/>
-    </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B185" s="1"/>
-    </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B186" s="1"/>
-    </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B187" s="1"/>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B188" s="1"/>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B189" s="1"/>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B190" s="1"/>
-    </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B191" s="1"/>
-    </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B192" s="1"/>
-    </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B193" s="1"/>
-    </row>
-    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B194" s="1"/>
-    </row>
-    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B195" s="1"/>
-    </row>
-    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B196" s="1"/>
-    </row>
-    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B197" s="1"/>
-    </row>
-    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B198" s="1"/>
-    </row>
-    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B199" s="1"/>
-    </row>
-    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B200" s="1"/>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B200">
-    <sortCondition descending="1" ref="B6"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9A4C79-82CA-4BF3-8CF0-A42D32042EC4}">
-  <dimension ref="A1:D50"/>
-  <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2019</v>
-      </c>
-      <c r="D2" s="3">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4">
-        <v>67.930134460146263</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="D3" s="4">
-        <v>55.154034599635715</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="4">
-        <v>54.422865772358897</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7.7142000000000002E-2</v>
-      </c>
-      <c r="D4" s="4">
-        <v>3.1551076475507958</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="4">
-        <v>51.874196341724712</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.372</v>
-      </c>
-      <c r="D5" s="4">
-        <v>5.6319177003723295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="4">
-        <v>48.78376973831292</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.112</v>
-      </c>
-      <c r="D6" s="4">
-        <v>3.3416341739058324</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="4">
-        <v>46.310440110633465</v>
-      </c>
-      <c r="C7" s="1">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.6619592592592591</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4">
-        <v>42.690670934685158</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.18</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2.1187915464671665</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="4">
-        <v>40.933380524003205</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.112</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.2050169994221624</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="4">
-        <v>37.80357401561308</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.28042940625000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="4">
-        <v>29.184731185530865</v>
-      </c>
-      <c r="C11" s="1">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1.1639085744788999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="4">
-        <v>28.808808649853312</v>
-      </c>
-      <c r="C12" s="1">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.5800768394649225</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="4">
-        <v>28.029657202706129</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.92359608895041967</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4">
-        <v>24.957625968211211</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.11</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.82471851851851841</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="4">
-        <v>24.19915495212669</v>
-      </c>
-      <c r="C15" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.57852048148148139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="4">
-        <v>23.426060338983973</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="D16" s="4">
-        <v>13.578799999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="4">
-        <v>20.970349597414291</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.40799999999999997</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1.9825185406134</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="4">
-        <v>20.519983638199051</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0.623</v>
-      </c>
-      <c r="D18" s="4">
-        <v>5.5428131458303209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="4">
-        <v>20.518964002216507</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.85225658584127795</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="4">
-        <v>19.655198810262576</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0.28699999999999998</v>
-      </c>
-      <c r="D20" s="4">
-        <v>5.2979588617104501</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="4">
-        <v>18.863590913688778</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1.9818461711964659</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="4">
-        <v>17.526765654825013</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2.734</v>
-      </c>
-      <c r="D22" s="4">
-        <v>15.807932888968995</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="4">
-        <v>15.615972357211408</v>
-      </c>
-      <c r="C23" s="1">
-        <v>4.0679999999999996</v>
-      </c>
-      <c r="D23" s="4">
-        <v>60.752171540493542</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="4">
-        <v>15.039183722225999</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="D24" s="4">
-        <v>5.4972580042428421</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="4">
-        <v>13.861384589203558</v>
-      </c>
-      <c r="C25" s="1">
-        <v>15.6</v>
-      </c>
-      <c r="D25" s="4">
-        <v>26.727593461374745</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="4">
-        <v>13.149106851576454</v>
-      </c>
-      <c r="C26" s="1">
-        <v>3.7240000000000002</v>
-      </c>
-      <c r="D26" s="4">
-        <v>17.476842102993885</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="4">
-        <v>12.441988834685356</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.4218140803669676</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="4">
-        <v>12.393707069492546</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="D28" s="4">
-        <v>7.9533552117448307</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="4">
-        <v>9.122894701715115</v>
-      </c>
-      <c r="C29" s="1">
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="D29" s="4">
-        <v>15.214920017147165</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="4">
-        <v>8.7262991641330387</v>
-      </c>
-      <c r="C30" s="1">
-        <v>69.626000000000005</v>
-      </c>
-      <c r="D30" s="4">
-        <v>544.20954952918362</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="4">
-        <v>8.2046387247601285</v>
-      </c>
-      <c r="C31" s="1">
-        <v>10.07</v>
-      </c>
-      <c r="D31" s="4">
-        <v>44.565751751798686</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="4">
-        <v>8.1907939958705605</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1.2669999999999999</v>
-      </c>
-      <c r="D32" s="4">
-        <v>14.048423918124824</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="4">
-        <v>8.0623293936444256</v>
-      </c>
-      <c r="C33" s="1">
-        <v>10.358000000000001</v>
-      </c>
-      <c r="D33" s="4">
-        <v>89.031619777110421</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="4">
-        <v>7.6027123016297669</v>
-      </c>
-      <c r="C34" s="1">
-        <v>0.876</v>
-      </c>
-      <c r="D34" s="4">
-        <v>24.952593909616546</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="4">
-        <v>7.3461562244860756</v>
-      </c>
-      <c r="C35" s="1">
-        <v>10.725</v>
-      </c>
-      <c r="D35" s="4">
-        <v>205.34883886842613</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="4">
-        <v>5.5386213839232239</v>
-      </c>
-      <c r="C36" s="1">
-        <v>10.286</v>
-      </c>
-      <c r="D36" s="4">
-        <v>239.53710912982544</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="4">
-        <v>5.2515834542103743</v>
-      </c>
-      <c r="C37" s="1">
-        <v>4.2190000000000003</v>
-      </c>
-      <c r="D37" s="4">
-        <v>66.787866841095592</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="4">
-        <v>5.2090756832364296</v>
-      </c>
-      <c r="C38" s="1">
-        <v>1.484</v>
-      </c>
-      <c r="D38" s="4">
-        <v>38.473723404255317</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="4">
-        <v>5.1634574951397969</v>
-      </c>
-      <c r="C39" s="1">
-        <v>0.35699999999999998</v>
-      </c>
-      <c r="D39" s="4">
-        <v>24.836710978851144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" s="4">
-        <f>AVERAGE(B3:B39)</f>
-        <v>22.387292669152441</v>
-      </c>
-      <c r="C41" s="1">
-        <f t="shared" ref="C41:D41" si="0">AVERAGE(C3:C39)</f>
-        <v>4.1493011351351354</v>
-      </c>
-      <c r="D41" s="4">
-        <f t="shared" si="0"/>
-        <v>41.851350825853245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="4">
-        <f>MEDIAN(B3:B39)</f>
-        <v>18.863590913688778</v>
-      </c>
-      <c r="C42" s="4">
-        <f t="shared" ref="C42:D42" si="1">MEDIAN(C3:C39)</f>
-        <v>0.49399999999999999</v>
-      </c>
-      <c r="D42" s="4">
-        <f t="shared" si="1"/>
-        <v>5.6319177003723295</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="10"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B45" s="4">
-        <v>64.756210402315816</v>
-      </c>
-      <c r="C45" s="1">
-        <v>5.8559999999999999</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1.1974200000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="4">
-        <v>60.207974676378726</v>
-      </c>
-      <c r="C46" s="1">
-        <v>4.1486000000000002E-2</v>
-      </c>
-      <c r="D46" s="4">
-        <v>1.0089999999999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="4">
-        <v>38.940448139497711</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1.4730999999999999E-2</v>
-      </c>
-      <c r="D47" s="4">
-        <v>0.37958518518518519</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="4">
-        <v>11.317765119694657</v>
-      </c>
-      <c r="C48" s="1">
-        <v>6.4173999999999995E-2</v>
-      </c>
-      <c r="D48" s="4">
-        <v>6.0201840000000004</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49" s="4">
-        <v>7.8640318001519294</v>
-      </c>
-      <c r="C49" s="1">
-        <v>0.16342400000000001</v>
-      </c>
-      <c r="D49" s="4">
-        <v>3.1017877094972</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="4">
-        <v>6.0610415390536456</v>
-      </c>
-      <c r="C50" s="1">
-        <v>0.27928399999999998</v>
-      </c>
-      <c r="D50" s="4">
-        <v>6.02336768898674</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5602254-0EAF-4023-AD37-78D369F7FDA1}">
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3442,35 +3058,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
     </row>
     <row r="4" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3765,12 +3381,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0320106B-1FDC-408D-A1CE-169E26EA0682}">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3784,16 +3400,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="47.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="15" t="s">
@@ -4042,182 +3658,1829 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9F6483-098D-4B3D-8661-531F940D7152}">
-  <dimension ref="A2:G11"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33FD584-3AA7-477E-8AE4-0DD69A91E032}">
+  <dimension ref="A1:B200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="4">
+        <v>7.0160379932140611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5.9485074187079601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="11">
+        <v>5.1204749911959739</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4">
+        <v>4.9184804413390042</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="4">
+        <v>4.3485991674098523</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="4">
+        <v>3.7569446794271428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3.3441612719013563</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3.2104974633661691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3.1652758935326522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2.8373919457960826</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B124" s="8"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B149" s="1"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B150" s="1"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B151" s="1"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B152" s="1"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B153" s="1"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B155" s="1"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B156" s="1"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B157" s="1"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B158" s="1"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B159" s="1"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B160" s="1"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B161" s="1"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B162" s="1"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B163" s="1"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B164" s="1"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B165" s="1"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B166" s="1"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B167" s="1"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B170" s="1"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B171" s="1"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B172" s="1"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B173" s="1"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B174" s="1"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B175" s="1"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B176" s="1"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B177" s="1"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B179" s="1"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B180" s="1"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B181" s="1"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B182" s="1"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B183" s="1"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B184" s="1"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B185" s="1"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B186" s="1"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B187" s="1"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B188" s="1"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B189" s="1"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B190" s="1"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B191" s="1"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B192" s="1"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B193" s="1"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B194" s="1"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B195" s="1"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B196" s="1"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B197" s="1"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B198" s="1"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B199" s="1"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B200" s="1"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B200">
+    <sortCondition descending="1" ref="B6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C674EB93-1C91-45A5-99C0-B244CA792153}">
+  <dimension ref="A1:K63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.5" customWidth="1"/>
+    <col min="9" max="9" width="7" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="17" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="47.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:11" ht="35.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="25">
+        <v>166</v>
+      </c>
+      <c r="D4" s="26">
+        <v>0.63907020000000003</v>
+      </c>
+      <c r="E4" s="26">
+        <v>2.4150040000000002</v>
+      </c>
+      <c r="F4" s="26">
+        <v>3.5700340000000002</v>
+      </c>
+      <c r="G4" s="26">
+        <v>5.8213100000000004</v>
+      </c>
+      <c r="H4" s="26">
+        <v>38.82432</v>
+      </c>
+      <c r="I4" s="26">
+        <v>5.2488530000000004</v>
+      </c>
+      <c r="J4" s="26">
+        <v>5.3424180000000003</v>
+      </c>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="25">
+        <v>36</v>
+      </c>
+      <c r="D5" s="26">
+        <v>1.6180239999999999</v>
+      </c>
+      <c r="E5" s="26">
+        <v>2.2325400000000002</v>
+      </c>
+      <c r="F5" s="26">
+        <v>3.4772910000000001</v>
+      </c>
+      <c r="G5" s="26">
+        <v>5.362387</v>
+      </c>
+      <c r="H5" s="26">
+        <v>28.063099999999999</v>
+      </c>
+      <c r="I5" s="26">
+        <v>4.6263139999999998</v>
+      </c>
+      <c r="J5" s="26">
+        <v>4.7286450000000002</v>
+      </c>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="25">
+        <v>130</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0.63907020000000003</v>
+      </c>
+      <c r="E6" s="26">
+        <v>2.5864020000000001</v>
+      </c>
+      <c r="F6" s="26">
+        <v>3.570897</v>
+      </c>
+      <c r="G6" s="26">
+        <v>6.0719820000000002</v>
+      </c>
+      <c r="H6" s="26">
+        <v>38.82432</v>
+      </c>
+      <c r="I6" s="26">
+        <v>5.4212480000000003</v>
+      </c>
+      <c r="J6" s="26">
+        <v>5.5046970000000002</v>
+      </c>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="25">
+        <v>166</v>
+      </c>
+      <c r="D8" s="26">
+        <v>1.7589520000000001</v>
+      </c>
+      <c r="E8" s="26">
+        <v>2.9341499999999998</v>
+      </c>
+      <c r="F8" s="26">
+        <v>9.6283049999999992</v>
+      </c>
+      <c r="G8" s="26">
+        <v>15.99492</v>
+      </c>
+      <c r="H8" s="26">
+        <v>87.464119999999994</v>
+      </c>
+      <c r="I8" s="26">
+        <v>14.149240000000001</v>
+      </c>
+      <c r="J8" s="26">
+        <v>13.394270000000001</v>
+      </c>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="25">
+        <v>36</v>
+      </c>
+      <c r="D9" s="26">
+        <v>4.4180580000000003</v>
+      </c>
+      <c r="E9" s="26">
+        <v>6.7185810000000004</v>
+      </c>
+      <c r="F9" s="26">
+        <v>9.3820099999999993</v>
+      </c>
+      <c r="G9" s="26">
+        <v>15.105420000000001</v>
+      </c>
+      <c r="H9" s="26">
+        <v>58.966819999999998</v>
+      </c>
+      <c r="I9" s="26">
+        <v>12.78407</v>
+      </c>
+      <c r="J9" s="26">
+        <v>10.198359999999999</v>
+      </c>
+      <c r="K9" s="13"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="25">
+        <v>130</v>
+      </c>
+      <c r="D10" s="26">
+        <v>1.7589520000000001</v>
+      </c>
+      <c r="E10" s="26">
+        <v>6.5943860000000001</v>
+      </c>
+      <c r="F10" s="26">
+        <v>9.6954930000000008</v>
+      </c>
+      <c r="G10" s="26">
+        <v>16.069520000000001</v>
+      </c>
+      <c r="H10" s="26">
+        <v>87.464119999999994</v>
+      </c>
+      <c r="I10" s="26">
+        <v>14.527290000000001</v>
+      </c>
+      <c r="J10" s="26">
+        <v>14.163</v>
+      </c>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J12"/>
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J13"/>
+      <c r="K13"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J14"/>
+      <c r="K14"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J21"/>
+      <c r="K21"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J22"/>
+      <c r="K22"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J23"/>
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J24"/>
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J25"/>
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J26"/>
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J28"/>
+      <c r="K28"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J29"/>
+      <c r="K29"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J30"/>
+      <c r="K30"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J31"/>
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J32"/>
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J33"/>
+      <c r="K33"/>
+    </row>
+    <row r="34" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J34"/>
+      <c r="K34"/>
+    </row>
+    <row r="35" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J35"/>
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J36"/>
+      <c r="K36"/>
+    </row>
+    <row r="37" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J37"/>
+      <c r="K37"/>
+    </row>
+    <row r="38" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J38"/>
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J39"/>
+      <c r="K39"/>
+    </row>
+    <row r="40" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J40"/>
+      <c r="K40"/>
+    </row>
+    <row r="41" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J41"/>
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J42"/>
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J43"/>
+      <c r="K43"/>
+    </row>
+    <row r="44" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J44"/>
+      <c r="K44"/>
+    </row>
+    <row r="45" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J45"/>
+      <c r="K45"/>
+    </row>
+    <row r="46" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J46"/>
+      <c r="K46"/>
+    </row>
+    <row r="47" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J47"/>
+      <c r="K47"/>
+    </row>
+    <row r="48" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J48"/>
+      <c r="K48"/>
+    </row>
+    <row r="49" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J49"/>
+      <c r="K49"/>
+    </row>
+    <row r="50" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J50"/>
+      <c r="K50"/>
+    </row>
+    <row r="51" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J51"/>
+      <c r="K51"/>
+    </row>
+    <row r="52" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J52"/>
+      <c r="K52"/>
+    </row>
+    <row r="53" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J53"/>
+      <c r="K53"/>
+    </row>
+    <row r="54" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J54"/>
+      <c r="K54"/>
+    </row>
+    <row r="55" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J55"/>
+      <c r="K55"/>
+    </row>
+    <row r="56" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J56"/>
+      <c r="K56"/>
+    </row>
+    <row r="57" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J57"/>
+      <c r="K57"/>
+    </row>
+    <row r="58" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J58"/>
+      <c r="K58"/>
+    </row>
+    <row r="59" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J59"/>
+      <c r="K59"/>
+    </row>
+    <row r="60" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J60"/>
+      <c r="K60"/>
+    </row>
+    <row r="61" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J61"/>
+      <c r="K61"/>
+    </row>
+    <row r="62" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J62"/>
+      <c r="K62"/>
+    </row>
+    <row r="63" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J63"/>
+      <c r="K63"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C013406C-EC10-8040-8782-84B22EAA646A}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="25">
+        <v>166</v>
+      </c>
+      <c r="D2" s="26">
+        <v>0.63907020000000003</v>
+      </c>
+      <c r="E2" s="26">
+        <v>2.4150040000000002</v>
+      </c>
+      <c r="F2" s="26">
+        <v>3.5700340000000002</v>
+      </c>
+      <c r="G2" s="26">
+        <v>5.8213100000000004</v>
+      </c>
+      <c r="H2" s="26">
+        <v>38.82432</v>
+      </c>
+      <c r="I2" s="26">
+        <v>5.2488530000000004</v>
+      </c>
+      <c r="J2" s="26">
+        <v>5.3424180000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="25">
+        <v>36</v>
+      </c>
+      <c r="D3" s="26">
+        <v>1.6180239999999999</v>
+      </c>
+      <c r="E3" s="26">
+        <v>2.2325400000000002</v>
+      </c>
+      <c r="F3" s="26">
+        <v>3.4772910000000001</v>
+      </c>
+      <c r="G3" s="26">
+        <v>5.362387</v>
+      </c>
+      <c r="H3" s="26">
+        <v>28.063099999999999</v>
+      </c>
+      <c r="I3" s="26">
+        <v>4.6263139999999998</v>
+      </c>
+      <c r="J3" s="26">
+        <v>4.7286450000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="25">
+        <v>130</v>
+      </c>
+      <c r="D4" s="26">
+        <v>0.63907020000000003</v>
+      </c>
+      <c r="E4" s="26">
+        <v>2.5864020000000001</v>
+      </c>
+      <c r="F4" s="26">
+        <v>3.570897</v>
+      </c>
+      <c r="G4" s="26">
+        <v>6.0719820000000002</v>
+      </c>
+      <c r="H4" s="26">
+        <v>38.82432</v>
+      </c>
+      <c r="I4" s="26">
+        <v>5.4212480000000003</v>
+      </c>
+      <c r="J4" s="26">
+        <v>5.5046970000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="25">
+        <v>166</v>
+      </c>
+      <c r="D5" s="26">
+        <v>1.7589520000000001</v>
+      </c>
+      <c r="E5" s="26">
+        <v>2.9341499999999998</v>
+      </c>
+      <c r="F5" s="26">
+        <v>9.6283049999999992</v>
+      </c>
+      <c r="G5" s="26">
+        <v>15.99492</v>
+      </c>
+      <c r="H5" s="26">
+        <v>87.464119999999994</v>
+      </c>
+      <c r="I5" s="26">
+        <v>14.149240000000001</v>
+      </c>
+      <c r="J5" s="26">
+        <v>13.394270000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="25">
+        <v>36</v>
+      </c>
+      <c r="D6" s="26">
+        <v>4.4180580000000003</v>
+      </c>
+      <c r="E6" s="26">
+        <v>6.7185810000000004</v>
+      </c>
+      <c r="F6" s="26">
+        <v>9.3820099999999993</v>
+      </c>
+      <c r="G6" s="26">
+        <v>15.105420000000001</v>
+      </c>
+      <c r="H6" s="26">
+        <v>58.966819999999998</v>
+      </c>
+      <c r="I6" s="26">
+        <v>12.78407</v>
+      </c>
+      <c r="J6" s="26">
+        <v>10.198359999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="25">
+        <v>130</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1.7589520000000001</v>
+      </c>
+      <c r="E7" s="26">
+        <v>6.5943860000000001</v>
+      </c>
+      <c r="F7" s="26">
+        <v>9.6954930000000008</v>
+      </c>
+      <c r="G7" s="26">
+        <v>16.069520000000001</v>
+      </c>
+      <c r="H7" s="26">
+        <v>87.464119999999994</v>
+      </c>
+      <c r="I7" s="26">
+        <v>14.527290000000001</v>
+      </c>
+      <c r="J7" s="26">
+        <v>14.163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB16FAD-61C9-1B49-BFA2-0618093FCB44}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="34">
+        <v>186</v>
+      </c>
+      <c r="D2" s="35">
+        <v>-55.2</v>
+      </c>
+      <c r="E2" s="35">
+        <v>-10.3</v>
+      </c>
+      <c r="F2" s="35">
+        <v>-7</v>
+      </c>
+      <c r="G2" s="35">
+        <v>-4.7</v>
+      </c>
+      <c r="H2" s="35">
+        <v>3.3</v>
+      </c>
+      <c r="I2" s="35">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="J2" s="35">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="34">
+        <v>37</v>
+      </c>
+      <c r="D3" s="35">
+        <v>-55.2</v>
+      </c>
+      <c r="E3" s="35">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F3" s="35">
+        <v>-6.1</v>
+      </c>
+      <c r="G3" s="35">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="H3" s="35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I3" s="35">
+        <v>-7.8</v>
+      </c>
+      <c r="J3" s="35">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="10">
-        <v>-4.7584939999999998</v>
-      </c>
-      <c r="C4" s="10">
-        <v>5.3715250000000001</v>
-      </c>
-      <c r="D4" s="10">
-        <v>-4.8007220000000004</v>
-      </c>
-      <c r="E4" s="10">
-        <v>-15.45575</v>
-      </c>
-      <c r="F4" s="10">
-        <v>9.3905700000000003</v>
-      </c>
-      <c r="G4" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="34">
+        <v>149</v>
+      </c>
+      <c r="D4" s="35">
+        <v>-38.299999999999997</v>
+      </c>
+      <c r="E4" s="35">
+        <v>-10.7</v>
+      </c>
+      <c r="F4" s="35">
+        <v>-7.1</v>
+      </c>
+      <c r="G4" s="35">
+        <v>-4.7</v>
+      </c>
+      <c r="H4" s="35">
+        <v>3.3</v>
+      </c>
+      <c r="I4" s="35">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="J4" s="35">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="10">
-        <v>2.5102600000000002</v>
-      </c>
-      <c r="C5" s="10">
-        <v>3.1506069999999999</v>
-      </c>
-      <c r="D5" s="10">
-        <v>1.8544849999999999</v>
-      </c>
-      <c r="E5" s="10">
-        <v>-4.2025220000000001</v>
-      </c>
-      <c r="F5" s="10">
-        <v>8.4722139999999992</v>
-      </c>
-      <c r="G5" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="34">
+        <v>36</v>
+      </c>
+      <c r="D5" s="35">
+        <v>-55.2</v>
+      </c>
+      <c r="E5" s="35">
+        <v>-18.8</v>
+      </c>
+      <c r="F5" s="35">
+        <v>-12.2</v>
+      </c>
+      <c r="G5" s="35">
+        <v>-10</v>
+      </c>
+      <c r="H5" s="35">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="I5" s="35">
+        <v>-15.6</v>
+      </c>
+      <c r="J5" s="35">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B6" s="10">
-        <v>1.36439</v>
-      </c>
-      <c r="C6" s="10">
-        <v>4.0988309999999997</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0.18954109999999999</v>
-      </c>
-      <c r="E6" s="10">
-        <v>-4.4756530000000003</v>
-      </c>
-      <c r="F6" s="10">
-        <v>17.131250000000001</v>
-      </c>
-      <c r="G6" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="34">
+        <v>6</v>
+      </c>
+      <c r="D6" s="35">
+        <v>-55.2</v>
+      </c>
+      <c r="E6" s="35">
+        <v>-12.1</v>
+      </c>
+      <c r="F6" s="35">
+        <v>-9.9</v>
+      </c>
+      <c r="G6" s="35">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="H6" s="35">
+        <v>-8</v>
+      </c>
+      <c r="I6" s="35">
+        <v>-17.2</v>
+      </c>
+      <c r="J6" s="35">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="10">
-        <v>-11.470890000000001</v>
-      </c>
-      <c r="C7" s="10">
-        <v>6.4548839999999998</v>
-      </c>
-      <c r="D7" s="10">
-        <v>-10.673719999999999</v>
-      </c>
-      <c r="E7" s="10">
-        <v>-23.69586</v>
-      </c>
-      <c r="F7" s="10">
-        <v>-0.96835139999999997</v>
-      </c>
-      <c r="G7" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="34">
+        <v>30</v>
+      </c>
+      <c r="D7" s="35">
+        <v>-38.299999999999997</v>
+      </c>
+      <c r="E7" s="35">
+        <v>-19</v>
+      </c>
+      <c r="F7" s="35">
+        <v>-15.7</v>
+      </c>
+      <c r="G7" s="35">
+        <v>-10.3</v>
+      </c>
+      <c r="H7" s="35">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="I7" s="35">
+        <v>-15.3</v>
+      </c>
+      <c r="J7" s="35">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="10">
-        <v>1.38619</v>
-      </c>
-      <c r="C8" s="10">
-        <v>2.0649359999999999</v>
-      </c>
-      <c r="D8" s="10">
-        <v>1.0368250000000001</v>
-      </c>
-      <c r="E8" s="10">
-        <v>-1.6213</v>
-      </c>
-      <c r="F8" s="10">
-        <v>7.4287510000000001</v>
-      </c>
-      <c r="G8" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="34">
+        <v>142</v>
+      </c>
+      <c r="D8" s="35">
+        <v>-16</v>
+      </c>
+      <c r="E8" s="35">
+        <v>-8.3000000000000007</v>
+      </c>
+      <c r="F8" s="35">
+        <v>-6.4</v>
+      </c>
+      <c r="G8" s="35">
+        <v>-4.5</v>
+      </c>
+      <c r="H8" s="35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I8" s="35">
+        <v>-6.6</v>
+      </c>
+      <c r="J8" s="35">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="10">
-        <v>1.4515629999999999</v>
-      </c>
-      <c r="C9" s="10">
-        <v>2.187506</v>
-      </c>
-      <c r="D9" s="10">
-        <v>0.80064999999999997</v>
-      </c>
-      <c r="E9" s="10">
-        <v>-2.7993000000000001</v>
-      </c>
-      <c r="F9" s="10">
-        <v>5.5223000000000004</v>
-      </c>
-      <c r="G9" s="13">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D11" s="10"/>
+        <v>129</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="31">
+        <v>31</v>
+      </c>
+      <c r="D9" s="35">
+        <v>-12.4</v>
+      </c>
+      <c r="E9" s="35">
+        <v>-7.6</v>
+      </c>
+      <c r="F9" s="35">
+        <v>-5.7</v>
+      </c>
+      <c r="G9" s="35">
+        <v>-4.3</v>
+      </c>
+      <c r="H9" s="35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I9" s="35">
+        <v>-5.9</v>
+      </c>
+      <c r="J9" s="35">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="31">
+        <v>108</v>
+      </c>
+      <c r="D10" s="35">
+        <v>-16</v>
+      </c>
+      <c r="E10" s="35">
+        <v>-8.6</v>
+      </c>
+      <c r="F10" s="35">
+        <v>-6.6</v>
+      </c>
+      <c r="G10" s="35">
+        <v>-4.5</v>
+      </c>
+      <c r="H10" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="I10" s="35">
+        <v>-6.8</v>
+      </c>
+      <c r="J10" s="35">
+        <v>3.6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>